<commit_message>
Updated with scaledILD files
</commit_message>
<xml_diff>
--- a/SubjectiveTest/Result.xlsx
+++ b/SubjectiveTest/Result.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\MATLAB\Thesis\SubjectiveTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\BinauralCue\SubjectiveTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0B25DE-5DCB-4E67-904E-118F3819102F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB05F399-A995-4205-91D4-FBCAD0097A3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vasudha" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
   <si>
     <t>Unprocessed</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>SCENE C</t>
+  </si>
+  <si>
+    <t>Repetition 1</t>
+  </si>
+  <si>
+    <t>Repetition 2</t>
+  </si>
+  <si>
+    <t>scaledILD0.2</t>
+  </si>
+  <si>
+    <t>scaledILD0.4</t>
+  </si>
+  <si>
+    <t>scaledILD0.6</t>
+  </si>
+  <si>
+    <t>scaledILD0.8</t>
+  </si>
+  <si>
+    <t>scaledILD1</t>
   </si>
 </sst>
 </file>
@@ -101,7 +122,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -109,17 +130,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,29 +451,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4E01D3-2816-41A4-9FC6-FE3474815303}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30:L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="16" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="2.140625" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="2.140625" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="2.140625" bestFit="true" customWidth="true"/>
-    <col min="6" max="6" width="2.140625" customWidth="true"/>
-    <col min="7" max="7" width="2.140625" customWidth="true"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
@@ -475,8 +494,26 @@
       <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -495,8 +532,23 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" x14ac:dyDescent="0.25">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -515,8 +567,23 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" x14ac:dyDescent="0.25">
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -535,8 +602,23 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" x14ac:dyDescent="0.25">
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -555,124 +637,270 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-    </row>
-    <row r="13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" x14ac:dyDescent="0.25">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -683,12 +911,31 @@
       <c r="E15" s="1">
         <v>0</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" x14ac:dyDescent="0.25">
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -699,12 +946,31 @@
       <c r="E16" s="1">
         <v>0</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" x14ac:dyDescent="0.25">
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -715,24 +981,533 @@
       <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed K2 to Scaled_ILD1
</commit_message>
<xml_diff>
--- a/SubjectiveTest/Result.xlsx
+++ b/SubjectiveTest/Result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\MATLAB\Thesis\SubjectiveTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/localadmin/Documents/GitHub/BinauralCue/SubjectiveTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74957D9-A207-45AB-AA39-A18DBE962555}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555AEF7F-7C7E-6345-A519-6166B3908E9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vasudha" sheetId="1" r:id="rId1"/>
@@ -482,31 +482,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4E01D3-2816-41A4-9FC6-FE3474815303}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" customWidth="1"/>
-    <col min="14" max="14" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5" customWidth="1"/>
+    <col min="5" max="5" width="3.1640625" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" customWidth="1"/>
+    <col min="8" max="8" width="6.5" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" customWidth="1"/>
+    <col min="14" max="14" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
@@ -535,12 +538,12 @@
         <v>19</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -563,7 +566,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -577,7 +580,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -597,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I4" s="1">
         <v>0</v>
@@ -611,7 +614,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -619,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -645,7 +648,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -656,7 +659,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -682,7 +685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="112" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -696,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -721,7 +724,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -735,7 +738,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -758,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
@@ -772,7 +775,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
@@ -783,7 +786,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -806,12 +809,12 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -840,7 +843,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
@@ -860,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I12" s="1">
         <v>0</v>
@@ -877,7 +880,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="112" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
@@ -894,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
@@ -916,7 +919,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -933,7 +936,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
@@ -967,7 +970,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -981,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -1004,7 +1007,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1021,7 +1024,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -1038,7 +1041,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="K18" s="1">
         <v>0</v>
@@ -1072,7 +1075,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
@@ -1109,7 +1112,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="112" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -1148,7 +1151,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1162,7 +1165,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1185,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I22" s="1">
         <v>0</v>
@@ -1199,7 +1202,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
@@ -1233,7 +1236,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
@@ -1267,7 +1270,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -1304,7 +1307,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="112" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
@@ -1321,10 +1324,10 @@
         <v>0</v>
       </c>
       <c r="G26" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H26" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="I26" s="1">
         <v>0</v>
@@ -1343,7 +1346,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1357,7 +1360,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1371,7 +1374,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1385,7 +1388,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1399,7 +1402,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1413,7 +1416,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1427,7 +1430,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1441,7 +1444,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1455,7 +1458,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1469,7 +1472,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1483,7 +1486,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>

</xml_diff>